<commit_message>
update EM v3 CSV
</commit_message>
<xml_diff>
--- a/_apidocs/entity-api/v1/v3_CSV_Response.xlsx
+++ b/_apidocs/entity-api/v1/v3_CSV_Response.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\E04TCK-XDVCFP1\RedirAE$\jyothirmayichavali\Desktop\PI34\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATTFINNELL\git\open-gsa-redesign\_apidocs\entity-api\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785C4DCE-67C6-4944-BACD-F22D026BC64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB31FCB2-5365-408B-ABF4-679E9D9917B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example6-Entity (3)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="381">
   <si>
     <t>samRegistered</t>
   </si>
@@ -1144,12 +1144,6 @@
     <t>SOMETHING@SAM.GOV</t>
   </si>
   <si>
-    <t>sourceType</t>
-  </si>
-  <si>
-    <t>SAM</t>
-  </si>
-  <si>
     <t>publicDisplayFlag</t>
   </si>
   <si>
@@ -1166,6 +1160,9 @@
   </si>
   <si>
     <t>ultimateParentEntity.evsSource</t>
+  </si>
+  <si>
+    <t>evsSource</t>
   </si>
 </sst>
 </file>
@@ -2017,47 +2014,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ML2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JO1" workbookViewId="0">
-      <selection activeCell="KI10" sqref="KI10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.1796875" style="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="19.28515625" style="1" customWidth="1"/>
-    <col min="16" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="26.7109375" style="1" customWidth="1"/>
-    <col min="22" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="40.5703125" style="1" customWidth="1"/>
-    <col min="28" max="29" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="1"/>
-    <col min="31" max="31" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.140625" style="1"/>
+    <col min="4" max="10" width="9.1796875" style="1"/>
+    <col min="11" max="11" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1796875" style="1"/>
+    <col min="15" max="15" width="19.26953125" style="1" customWidth="1"/>
+    <col min="16" max="20" width="9.1796875" style="1"/>
+    <col min="21" max="21" width="26.7265625" style="1" customWidth="1"/>
+    <col min="22" max="25" width="9.1796875" style="1"/>
+    <col min="26" max="26" width="40.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="40.54296875" style="1" customWidth="1"/>
+    <col min="28" max="29" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.1796875" style="1"/>
+    <col min="31" max="31" width="42.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.1796875" style="1"/>
     <col min="34" max="34" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.140625" style="1"/>
-    <col min="37" max="37" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.5703125" style="1" customWidth="1"/>
-    <col min="40" max="49" width="9.140625" style="1"/>
-    <col min="50" max="50" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="27.5703125" style="1" customWidth="1"/>
-    <col min="52" max="53" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="61" width="9.140625" style="1"/>
-    <col min="62" max="62" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="38.42578125" style="1" customWidth="1"/>
-    <col min="64" max="64" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="290" width="9.140625" style="1"/>
+    <col min="35" max="36" width="9.1796875" style="1"/>
+    <col min="37" max="37" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="33.54296875" style="1" customWidth="1"/>
+    <col min="40" max="49" width="9.1796875" style="1"/>
+    <col min="50" max="50" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27.54296875" style="1" customWidth="1"/>
+    <col min="52" max="53" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="61" width="9.1796875" style="1"/>
+    <col min="62" max="62" width="38.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="38.453125" style="1" customWidth="1"/>
+    <col min="64" max="64" width="32.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="290" width="9.1796875" style="1"/>
     <col min="291" max="291" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="292" max="16384" width="9.140625" style="1"/>
+    <col min="292" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:350" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:350" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2091,8 +2088,8 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>374</v>
+      <c r="L1" t="s">
+        <v>380</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -2116,7 +2113,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -2137,7 +2134,7 @@
         <v>23</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>24</v>
@@ -2173,7 +2170,7 @@
         <v>34</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>35</v>
@@ -2209,7 +2206,7 @@
         <v>45</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>46</v>
@@ -2245,7 +2242,7 @@
         <v>56</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>57</v>
@@ -3109,7 +3106,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:350" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:350" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>344</v>
       </c>
@@ -3144,7 +3141,7 @@
         <v>351</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M2" s="2">
         <v>44379</v>
@@ -3189,7 +3186,7 @@
         <v>346</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>346</v>
@@ -3225,7 +3222,7 @@
         <v>346</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>346</v>
@@ -3261,7 +3258,7 @@
         <v>346</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AZ2" s="1" t="s">
         <v>346</v>
@@ -3297,7 +3294,7 @@
         <v>346</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="BL2" s="1" t="s">
         <v>346</v>

</xml_diff>